<commit_message>
Fixed some bugs with title of graph and theoData speed not being correct
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Mechanism/OTIS_Four_Bar/RMSE_Results/E/AngVel/sample1_csv/RMSE.xlsx
+++ b/Mechanisms/Four_Bar_Mechanism/OTIS_Four_Bar/RMSE_Results/E/AngVel/sample1_csv/RMSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teachinglab\Desktop\PMKS_Verification\Mechanisms\Four_Bar_Mechanism\OTIS_Four_Bar\RMSE_Results\E\AngVel\sample1_csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3881937-AB22-4B30-B72A-36AAF9D2879D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FCD0F1-DF2E-4E6A-9A8A-D2FB15B24AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7095" yWindow="1770" windowWidth="21600" windowHeight="11295" xr2:uid="{7741F1CB-DE59-498D-BBF3-9DA30E3C3875}"/>
+    <workbookView xWindow="7095" yWindow="1770" windowWidth="21600" windowHeight="11295" xr2:uid="{6099144F-54B4-4E34-8AFB-382062D1F77D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56573BCB-2CD7-45D6-8122-D843E0BB63EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829EFD44-21A6-44B1-9899-3E586ECC7BCB}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>